<commit_message>
Preço de compra e dash de lucro
</commit_message>
<xml_diff>
--- a/arquivos_processados/dados_finais.xlsx
+++ b/arquivos_processados/dados_finais.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M27"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1954,6 +1954,21 @@
         </is>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr"/>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>